<commit_message>
Updated CHE_grids model - 2025-08-19 17:28
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/Sets-vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18866FEF-25F1-4AA0-BCBB-B89156DE0250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EE0CFFA-C5EC-4C2D-B723-10AA69EF548F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1474,7 +1474,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDF61642-2F7D-5778-0E84-8D76C657434F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8733D68B-7E09-2164-8B8C-0BDB315A3AAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2256,7 +2256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5ADF667-A23B-46F1-8863-848AB078EF0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEA33E6-3DEC-47A8-8D97-DB603AF671B3}">
   <dimension ref="A1:H159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-21 13:24
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/Sets-vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D77687CC-B3D8-4D9D-940E-53810125527E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{383B9F43-44E1-4687-8B04-7326306684E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1624,7 +1624,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6804F898-504A-74AB-5746-43A219662AB1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00DB4FF8-E0BE-222C-5673-15D3960F4CA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2406,7 +2406,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CD7862-61F6-4D70-B670-E59E9F112877}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D26B71-DBC1-44EF-89E9-1636451A520E}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-23 15:16
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/Sets-vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C543E6B-EE78-482C-B507-7E10E4601001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE9525A5-7D3B-4006-AFEB-DD7DA1610C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1624,7 +1624,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE3655DC-0530-178B-2ED6-54B0DE29A907}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A48C11-1507-0080-E659-7CD36B1CE48A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2406,7 +2406,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1102EA1-6786-41DF-8177-4458D84BE7FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4047A5D2-E1A4-4372-832D-6197410D1130}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-31 21:16
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/Sets-vervestacks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr updateLinks="never" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5905EE06-F533-4D61-9A2C-E0CAFAD0106B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72A174DE-F721-412E-8406-7330339FBFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1288,6 +1288,54 @@
     <t>elc*CHE_0001</t>
   </si>
   <si>
+    <t>rez_CHE_2</t>
+  </si>
+  <si>
+    <t>elc*CHE_0002</t>
+  </si>
+  <si>
+    <t>rez_CHE_3</t>
+  </si>
+  <si>
+    <t>elc*CHE_0003</t>
+  </si>
+  <si>
+    <t>rez_CHE_4</t>
+  </si>
+  <si>
+    <t>elc*CHE_0004</t>
+  </si>
+  <si>
+    <t>rez_CHE_5</t>
+  </si>
+  <si>
+    <t>elc*CHE_0005</t>
+  </si>
+  <si>
+    <t>rez_CHE_6</t>
+  </si>
+  <si>
+    <t>elc*CHE_0006</t>
+  </si>
+  <si>
+    <t>rez_CHE_7</t>
+  </si>
+  <si>
+    <t>elc*CHE_0007</t>
+  </si>
+  <si>
+    <t>rez_CHE_8</t>
+  </si>
+  <si>
+    <t>elc*CHE_0008</t>
+  </si>
+  <si>
+    <t>rez_CHE_9</t>
+  </si>
+  <si>
+    <t>elc*CHE_0009</t>
+  </si>
+  <si>
     <t>rez_CHE_10</t>
   </si>
   <si>
@@ -1342,12 +1390,6 @@
     <t>elc*CHE_0019</t>
   </si>
   <si>
-    <t>rez_CHE_2</t>
-  </si>
-  <si>
-    <t>elc*CHE_0002</t>
-  </si>
-  <si>
     <t>rez_CHE_20</t>
   </si>
   <si>
@@ -1382,48 +1424,6 @@
   </si>
   <si>
     <t>elc*CHE_0025</t>
-  </si>
-  <si>
-    <t>rez_CHE_3</t>
-  </si>
-  <si>
-    <t>elc*CHE_0003</t>
-  </si>
-  <si>
-    <t>rez_CHE_4</t>
-  </si>
-  <si>
-    <t>elc*CHE_0004</t>
-  </si>
-  <si>
-    <t>rez_CHE_5</t>
-  </si>
-  <si>
-    <t>elc*CHE_0005</t>
-  </si>
-  <si>
-    <t>rez_CHE_6</t>
-  </si>
-  <si>
-    <t>elc*CHE_0006</t>
-  </si>
-  <si>
-    <t>rez_CHE_7</t>
-  </si>
-  <si>
-    <t>elc*CHE_0007</t>
-  </si>
-  <si>
-    <t>rez_CHE_8</t>
-  </si>
-  <si>
-    <t>elc*CHE_0008</t>
-  </si>
-  <si>
-    <t>rez_CHE_9</t>
-  </si>
-  <si>
-    <t>elc*CHE_0009</t>
   </si>
   <si>
     <t>VERVESTACKS - the open USE platform · Powered by data · Shaped by vision · Guided by intuition · Fueled by passion</t>
@@ -1624,7 +1624,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00499DBE-722A-F665-37C6-C6A5E3C1E09D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CCE5213-9983-1D4B-3649-F1311FFC3CD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2406,7 +2406,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2FFF841-062C-467F-8A09-5F6C5CA37A98}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049D828A-1378-405C-862A-A5176E21DB07}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>